<commit_message>
update for release to ISO addressing #30, #28, #27, #26, #24, #23, #21, #20, #19, #18, #17, #13, #12, #11, #10, #9, #6, #4, #3, #2, #1
</commit_message>
<xml_diff>
--- a/21838-2/bfo-2020-iris.xlsx
+++ b/21838-2/bfo-2020-iris.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Implication/Users/alanr/repos/bfo-theory/lsw-src/version/4/iso extras/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanr/repos/bfo-theory/lsw-src/version/11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6153F7E2-5B65-6148-AE60-9BC053B0DF42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85E34169-0F0F-5A4B-B46B-B9B036ED9868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52580" yWindow="1760" windowWidth="27240" windowHeight="16440" xr2:uid="{C48F8E80-8F15-5048-A0BD-CC939EC662BE}"/>
+    <workbookView xWindow="57900" yWindow="5640" windowWidth="32120" windowHeight="19600" xr2:uid="{C48F8E80-8F15-5048-A0BD-CC939EC662BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -258,9 +258,6 @@
     <t>http://purl.obolibrary.org/obo/BFO_0000217</t>
   </si>
   <si>
-    <t>spatially projects onto at</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000237</t>
   </si>
   <si>
@@ -282,9 +279,6 @@
     <t>http://purl.obolibrary.org/obo/BFO_0000211</t>
   </si>
   <si>
-    <t>occupies spatial region at</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000236</t>
   </si>
   <si>
@@ -324,9 +318,6 @@
     <t>http://purl.obolibrary.org/obo/BFO_0000166</t>
   </si>
   <si>
-    <t>participates in at</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000249</t>
   </si>
   <si>
@@ -342,9 +333,6 @@
     <t>http://purl.obolibrary.org/obo/BFO_0000167</t>
   </si>
   <si>
-    <t>has participant at</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000248</t>
   </si>
   <si>
@@ -372,9 +360,6 @@
     <t>http://purl.obolibrary.org/obo/BFO_0000082</t>
   </si>
   <si>
-    <t>located in at</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000238</t>
   </si>
   <si>
@@ -390,9 +375,6 @@
     <t>http://purl.obolibrary.org/obo/BFO_0000170</t>
   </si>
   <si>
-    <t>has location at</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000239</t>
   </si>
   <si>
@@ -420,9 +402,6 @@
     <t>http://purl.obolibrary.org/obo/BFO_0000219</t>
   </si>
   <si>
-    <t>generically depends on at</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000244</t>
   </si>
   <si>
@@ -438,9 +417,6 @@
     <t>http://purl.obolibrary.org/obo/BFO_0000220</t>
   </si>
   <si>
-    <t>is carrier of at</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000245</t>
   </si>
   <si>
@@ -492,9 +468,6 @@
     <t>http://purl.obolibrary.org/obo/BFO_0000164</t>
   </si>
   <si>
-    <t>concretizes at</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000246</t>
   </si>
   <si>
@@ -510,9 +483,6 @@
     <t>http://purl.obolibrary.org/obo/BFO_0000165</t>
   </si>
   <si>
-    <t>is concretized by at</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000247</t>
   </si>
   <si>
@@ -528,9 +498,6 @@
     <t>http://purl.obolibrary.org/obo/BFO_0000173</t>
   </si>
   <si>
-    <t>member part of at</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000234</t>
   </si>
   <si>
@@ -546,9 +513,6 @@
     <t>http://purl.obolibrary.org/obo/BFO_0000172</t>
   </si>
   <si>
-    <t>has member part at</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000235</t>
   </si>
   <si>
@@ -600,9 +564,6 @@
     <t>http://purl.obolibrary.org/obo/BFO_0000177</t>
   </si>
   <si>
-    <t>continuant part of at</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000230</t>
   </si>
   <si>
@@ -618,9 +579,6 @@
     <t>http://purl.obolibrary.org/obo/BFO_0000110</t>
   </si>
   <si>
-    <t>has continuant part at</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000231</t>
   </si>
   <si>
@@ -660,9 +618,6 @@
     <t>http://purl.obolibrary.org/obo/BFO_0000113</t>
   </si>
   <si>
-    <t>has material basis at</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000242</t>
   </si>
   <si>
@@ -678,9 +633,6 @@
     <t>http://purl.obolibrary.org/obo/BFO_0000163</t>
   </si>
   <si>
-    <t>material basis of at</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000243</t>
   </si>
   <si>
@@ -696,9 +648,6 @@
     <t>http://purl.obolibrary.org/obo/BFO_0000137</t>
   </si>
   <si>
-    <t>proper continuant part of at</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000232</t>
   </si>
   <si>
@@ -714,9 +663,6 @@
     <t>http://purl.obolibrary.org/obo/BFO_0000111</t>
   </si>
   <si>
-    <t>has proper continuant part at</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000233</t>
   </si>
   <si>
@@ -726,9 +672,6 @@
     <t>IRI</t>
   </si>
   <si>
-    <t>instance of at</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000193</t>
   </si>
   <si>
@@ -748,6 +691,63 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/BFO_0000054</t>
+  </si>
+  <si>
+    <t xml:space="preserve">concretizes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">continuant part of </t>
+  </si>
+  <si>
+    <t xml:space="preserve">generically depends on </t>
+  </si>
+  <si>
+    <t xml:space="preserve">has continuant part </t>
+  </si>
+  <si>
+    <t xml:space="preserve">has location </t>
+  </si>
+  <si>
+    <t xml:space="preserve">has material basis </t>
+  </si>
+  <si>
+    <t xml:space="preserve">has member part </t>
+  </si>
+  <si>
+    <t xml:space="preserve">has participant </t>
+  </si>
+  <si>
+    <t xml:space="preserve">has proper continuant part </t>
+  </si>
+  <si>
+    <t xml:space="preserve">instance of </t>
+  </si>
+  <si>
+    <t xml:space="preserve">is carrier of </t>
+  </si>
+  <si>
+    <t xml:space="preserve">is concretized by </t>
+  </si>
+  <si>
+    <t xml:space="preserve">located in </t>
+  </si>
+  <si>
+    <t xml:space="preserve">material basis of </t>
+  </si>
+  <si>
+    <t xml:space="preserve">member part of </t>
+  </si>
+  <si>
+    <t xml:space="preserve">occupies spatial region </t>
+  </si>
+  <si>
+    <t xml:space="preserve">participates in </t>
+  </si>
+  <si>
+    <t xml:space="preserve">proper continuant part of </t>
+  </si>
+  <si>
+    <t xml:space="preserve">spatially projects onto </t>
   </si>
 </sst>
 </file>
@@ -1122,8 +1122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94AE8AB0-CAE9-1443-A03B-84C2C1764257}">
   <dimension ref="A1:B120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="A99" sqref="A99"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1133,42 +1133,42 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>230</v>
+        <v>212</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>154</v>
+        <v>221</v>
       </c>
       <c r="B3" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -1189,26 +1189,26 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>190</v>
+        <v>222</v>
       </c>
       <c r="B8" t="s">
-        <v>191</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="B9" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="B10" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -1229,18 +1229,18 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>234</v>
+        <v>215</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>235</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
@@ -1277,10 +1277,10 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="B19" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -1301,234 +1301,234 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>130</v>
+        <v>223</v>
       </c>
       <c r="B22" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B23" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="B24" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>196</v>
+        <v>224</v>
       </c>
       <c r="B25" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="B26" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>192</v>
+        <v>179</v>
       </c>
       <c r="B27" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="B28" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="B29" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B30" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>120</v>
+        <v>225</v>
       </c>
       <c r="B31" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B32" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="B34" t="s">
-        <v>211</v>
+        <v>196</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="B35" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="B36" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>172</v>
+        <v>227</v>
       </c>
       <c r="B37" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="B38" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="B39" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="B40" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>104</v>
+        <v>228</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B43" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B44" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>226</v>
+        <v>209</v>
       </c>
       <c r="B45" t="s">
-        <v>227</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>224</v>
+        <v>207</v>
       </c>
       <c r="B46" t="s">
-        <v>225</v>
+        <v>208</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="B47" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B48" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>238</v>
+        <v>219</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="B50" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
@@ -1541,10 +1541,10 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="B52" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
@@ -1565,122 +1565,122 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="B55" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>136</v>
+        <v>231</v>
       </c>
       <c r="B57" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="B58" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B59" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>160</v>
+        <v>232</v>
       </c>
       <c r="B60" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B61" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B62" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="B63" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>114</v>
+        <v>233</v>
       </c>
       <c r="B64" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B65" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B66" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="B67" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>214</v>
+        <v>199</v>
       </c>
       <c r="B68" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>212</v>
+        <v>197</v>
       </c>
       <c r="B69" t="s">
-        <v>213</v>
+        <v>198</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
@@ -1693,26 +1693,26 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>166</v>
+        <v>235</v>
       </c>
       <c r="B71" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B72" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B73" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
@@ -1733,42 +1733,42 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>84</v>
+        <v>236</v>
       </c>
       <c r="B76" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
+        <v>81</v>
+      </c>
+      <c r="B77" t="s">
         <v>82</v>
-      </c>
-      <c r="B77" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" t="s">
         <v>80</v>
-      </c>
-      <c r="B78" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B79" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
+        <v>77</v>
+      </c>
+      <c r="B80" t="s">
         <v>78</v>
-      </c>
-      <c r="B80" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
@@ -1781,18 +1781,18 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="B82" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B83" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
@@ -1813,42 +1813,42 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>98</v>
+        <v>237</v>
       </c>
       <c r="B86" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B87" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B88" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="B89" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="B90" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
@@ -1869,42 +1869,42 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>222</v>
+        <v>238</v>
       </c>
       <c r="B93" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="B94" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="B95" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="B96" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B97" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
@@ -1925,10 +1925,10 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>236</v>
+        <v>217</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
@@ -1965,10 +1965,10 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
+        <v>239</v>
+      </c>
+      <c r="B105" t="s">
         <v>76</v>
-      </c>
-      <c r="B105" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
@@ -2005,18 +2005,18 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="B110" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="B111" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
@@ -2037,10 +2037,10 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="B114" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
@@ -2053,10 +2053,10 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B116" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
@@ -2093,7 +2093,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:B121" xr:uid="{69516A0C-6BEB-384F-AF30-1813F00836B8}">
-    <sortState ref="A2:B121">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B121">
       <sortCondition ref="A1:A121"/>
     </sortState>
   </autoFilter>

</xml_diff>